<commit_message>
Till 22-Jun-2021 Fro Vrushali
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rent It\Documents\RTA_FrameworkTemplate\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rent It\Documents\Metrics_Alert_project\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="99">
   <si>
     <t>Name</t>
   </si>
@@ -284,9 +284,6 @@
     <t>ProjectName</t>
   </si>
   <si>
-    <t>Test Suit</t>
-  </si>
-  <si>
     <t>Suit Name</t>
   </si>
   <si>
@@ -315,6 +312,15 @@
   </si>
   <si>
     <t>Test_Metrics_Alert</t>
+  </si>
+  <si>
+    <t>Download_file_path</t>
+  </si>
+  <si>
+    <t>C:\Users\Rent It\Documents\Metrics_Alert_project\Data\Temp\</t>
+  </si>
+  <si>
+    <t>Metrics_Alert_Test Suit</t>
   </si>
 </sst>
 </file>
@@ -372,7 +378,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -382,6 +388,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -402,7 +414,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -431,6 +443,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -746,10 +763,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1013"/>
+  <dimension ref="A1:Z1014"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -851,10 +868,10 @@
         <v>30</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C7" t="s">
         <v>94</v>
-      </c>
-      <c r="C7" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
@@ -969,266 +986,273 @@
       <c r="A26" s="5"/>
       <c r="B26" s="9"/>
     </row>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A27" s="12"/>
-      <c r="B27" s="13"/>
-      <c r="C27" s="10"/>
+    <row r="27" spans="1:3" s="18" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A27" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
-      <c r="B28" s="9"/>
+      <c r="A28" s="12"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="10"/>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A29" s="5" t="s">
+      <c r="B29" s="9"/>
+    </row>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A30" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B29" s="9"/>
-    </row>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A30" s="5"/>
       <c r="B30" s="9"/>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A31" s="5" t="s">
+      <c r="A31" s="5"/>
+      <c r="B31" s="9"/>
+    </row>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A32" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B31" s="9"/>
-    </row>
-    <row r="32" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A32" s="5"/>
       <c r="B32" s="9"/>
     </row>
     <row r="33" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A33" s="5" t="s">
+      <c r="A33" s="5"/>
+      <c r="B33" s="9"/>
+    </row>
+    <row r="34" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A34" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B33" s="9"/>
-    </row>
-    <row r="34" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A34" s="5"/>
       <c r="B34" s="9"/>
     </row>
     <row r="35" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A35" s="5" t="s">
+      <c r="A35" s="5"/>
+      <c r="B35" s="9"/>
+    </row>
+    <row r="36" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A36" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B35" s="9"/>
-    </row>
-    <row r="36" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A36" s="5"/>
       <c r="B36" s="9"/>
     </row>
     <row r="37" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A37" s="6" t="s">
+      <c r="A37" s="5"/>
+      <c r="B37" s="9"/>
+    </row>
+    <row r="38" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A38" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B37" s="7">
+      <c r="B38" s="7">
         <v>0</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C38" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A38" s="10"/>
-      <c r="B38" s="10"/>
-      <c r="C38" s="10"/>
-    </row>
-    <row r="39" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="40" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A40" s="5" t="s">
+    <row r="39" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A39" s="10"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
+    </row>
+    <row r="40" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="41" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A41" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B40" s="5"/>
-      <c r="C40" t="s">
+      <c r="B41" s="5"/>
+      <c r="C41" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A41" s="5"/>
-      <c r="B41" s="5"/>
-    </row>
     <row r="42" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A42" s="5" t="s">
+      <c r="A42" s="5"/>
+      <c r="B42" s="5"/>
+    </row>
+    <row r="43" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A43" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B42" s="5"/>
-      <c r="C42" t="s">
+      <c r="B43" s="5"/>
+      <c r="C43" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A43" s="5"/>
-      <c r="B43" s="5"/>
-    </row>
     <row r="44" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A44" s="5" t="s">
+      <c r="A44" s="5"/>
+      <c r="B44" s="5"/>
+    </row>
+    <row r="45" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A45" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B44" s="11"/>
-      <c r="C44" t="s">
+      <c r="B45" s="11"/>
+      <c r="C45" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="46" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A46" s="10"/>
-      <c r="B46" s="10"/>
-      <c r="C46" s="10"/>
-    </row>
-    <row r="47" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="48" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A48" t="s">
+    <row r="46" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="47" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A47" s="10"/>
+      <c r="B47" s="10"/>
+      <c r="C47" s="10"/>
+    </row>
+    <row r="48" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="49" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A49" t="s">
         <v>59</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="50" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A50" t="s">
+    <row r="50" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="51" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A51" t="s">
         <v>76</v>
       </c>
-      <c r="B50" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="C50" t="s">
+      <c r="B51" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="C51" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="52" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A52" t="s">
+    <row r="52" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="53" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A53" t="s">
         <v>78</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" t="s">
+        <v>98</v>
+      </c>
+      <c r="C53" t="s">
         <v>86</v>
       </c>
-      <c r="C52" t="s">
+    </row>
+    <row r="54" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="55" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A55" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="57" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A57" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="59" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A59" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="61" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A61" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="63" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A63" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="65" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A65" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="67" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A67" t="s">
+        <v>67</v>
+      </c>
+      <c r="B67" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="69" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A69" s="10"/>
+      <c r="B69" s="10"/>
+      <c r="C69" s="10"/>
+    </row>
+    <row r="70" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="71" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A71" t="s">
+        <v>69</v>
+      </c>
+      <c r="B71" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="54" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A54" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="56" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A56" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="58" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A58" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="60" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A60" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="62" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A62" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="64" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A64" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="66" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A66" t="s">
-        <v>67</v>
-      </c>
-      <c r="B66" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="68" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A68" s="10"/>
-      <c r="B68" s="10"/>
-      <c r="C68" s="10"/>
-    </row>
-    <row r="69" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="70" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A70" t="s">
-        <v>69</v>
-      </c>
-      <c r="B70" t="s">
+    <row r="72" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="73" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A73" t="s">
+        <v>70</v>
+      </c>
+      <c r="B73" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="72" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A72" t="s">
-        <v>70</v>
-      </c>
-      <c r="B72" t="s">
+    <row r="74" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="75" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A75" t="s">
+        <v>71</v>
+      </c>
+      <c r="B75" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="74" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A74" t="s">
-        <v>71</v>
-      </c>
-      <c r="B74" t="s">
+    <row r="76" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="77" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A77" t="s">
+        <v>72</v>
+      </c>
+      <c r="B77" s="14" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="79" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A79" t="s">
+        <v>73</v>
+      </c>
+      <c r="B79" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="76" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A76" t="s">
-        <v>72</v>
-      </c>
-      <c r="B76" s="14" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="78" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A78" t="s">
-        <v>73</v>
-      </c>
-      <c r="B78" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="80" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A80" t="s">
+    <row r="80" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="81" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A81" t="s">
         <v>74</v>
       </c>
-      <c r="B80">
+      <c r="B81">
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="82" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A82" s="10"/>
-      <c r="B82" s="10"/>
-      <c r="C82" s="10"/>
-    </row>
-    <row r="83" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="84" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A84" t="s">
+    <row r="82" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="83" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A83" s="10"/>
+      <c r="B83" s="10"/>
+      <c r="C83" s="10"/>
+    </row>
+    <row r="84" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="85" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A85" t="s">
         <v>75</v>
       </c>
-      <c r="B84">
+      <c r="B85">
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="86" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="87" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="88" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2157,6 +2181,7 @@
     <row r="1011" ht="14.25" customHeight="1"/>
     <row r="1012" ht="14.25" customHeight="1"/>
     <row r="1013" ht="14.25" customHeight="1"/>
+    <row r="1014" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2168,7 +2193,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -3300,7 +3325,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
File  Name: Config.xlsx Description: Updated Temp folder path Date: 30 June 2021 Developer: Snehalata
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rent It\Documents\Metrics_Alert_project\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\UiPath\MatrixAlertAutomation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11760"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -317,16 +317,16 @@
     <t>Download_file_path</t>
   </si>
   <si>
-    <t>C:\Users\Rent It\Documents\Metrics_Alert_project\Data\Temp\</t>
-  </si>
-  <si>
     <t>Metrics_Alert_Test Suit</t>
+  </si>
+  <si>
+    <t>C:\Users\HP\Documents\UiPath\MatrixAlertAutomation\Data\Temp\</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="8">
     <font>
       <sz val="11"/>
@@ -765,16 +765,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1014"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="88.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="88.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -851,7 +851,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="28.8">
+    <row r="5" spans="1:26" ht="30">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -991,7 +991,7 @@
         <v>96</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
@@ -1127,7 +1127,7 @@
         <v>78</v>
       </c>
       <c r="B53" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C53" t="s">
         <v>86</v>
@@ -2197,12 +2197,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2239,7 +2239,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -3309,12 +3309,12 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
Description : modification in test workflows after dry runs Developer Name : Vrushali Date : 05-Jul-2021
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\UiPath\MatrixAlertAutomation\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rent It\Documents\UiPath\MatrixAlertAutomation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="101">
   <si>
     <t>Name</t>
   </si>
@@ -320,13 +320,19 @@
     <t>Metrics_Alert_Test Suit</t>
   </si>
   <si>
-    <t>C:\Users\HP\Documents\UiPath\MatrixAlertAutomation\Data\Temp\</t>
+    <t>C:\Users\Rent It\Documents\UiPath\MatrixAlertAutomation\Data\Temp\</t>
+  </si>
+  <si>
+    <t>Upload_File_path</t>
+  </si>
+  <si>
+    <t>C:\Users\Rent It\Documents\Metrics_Alert_project\Data\Capture</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8">
     <font>
       <sz val="11"/>
@@ -414,7 +420,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -448,6 +454,10 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -765,16 +775,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1014"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="1" max="1" width="43.5546875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="88.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="88.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -851,7 +861,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="30">
+    <row r="5" spans="1:26" ht="28.8">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1000,7 +1010,12 @@
       <c r="C28" s="10"/>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
-      <c r="B29" s="9"/>
+      <c r="A29" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="B29" s="20" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
       <c r="A30" s="5" t="s">
@@ -2197,12 +2212,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2239,7 +2254,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="28.8">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -3309,12 +3324,12 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.88671875" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" customWidth="1"/>
+    <col min="3" max="3" width="60.33203125" customWidth="1"/>
+    <col min="4" max="26" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
Folder Name: Data Description: Test Data Updated Date: 5 July 2021 Developer: Snehalata
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rent It\Documents\UiPath\MatrixAlertAutomation\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\UiPath\MatrixAlertAutomation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11760"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -320,19 +320,19 @@
     <t>Metrics_Alert_Test Suit</t>
   </si>
   <si>
-    <t>C:\Users\Rent It\Documents\UiPath\MatrixAlertAutomation\Data\Temp\</t>
-  </si>
-  <si>
     <t>Upload_File_path</t>
   </si>
   <si>
-    <t>C:\Users\Rent It\Documents\Metrics_Alert_project\Data\Capture</t>
+    <t>C:\Users\HP\Documents\UiPath\MatrixAlertAutomation\Data\Temp\</t>
+  </si>
+  <si>
+    <t>C:\Users\HP\Documents\UiPath\MatrixAlertAutomation\Data\Capture</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="8">
     <font>
       <sz val="11"/>
@@ -776,15 +776,15 @@
   <dimension ref="A1:Z1014"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="88.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="88.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -861,7 +861,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="28.8">
+    <row r="5" spans="1:26" ht="30">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1001,7 +1001,7 @@
         <v>96</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
@@ -1011,7 +1011,7 @@
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B29" s="20" t="s">
         <v>100</v>
@@ -2212,12 +2212,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2254,7 +2254,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -3324,12 +3324,12 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
Description : updation of Exception handling and retry mechanics and according to best practices Developer Name : Vrushali Date : 07-Jul-2021
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\UiPath\MatrixAlertAutomation\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rent It\Documents\UiPath\MatrixAlertAutomation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -323,16 +323,16 @@
     <t>Upload_File_path</t>
   </si>
   <si>
-    <t>C:\Users\HP\Documents\UiPath\MatrixAlertAutomation\Data\Temp\</t>
-  </si>
-  <si>
-    <t>C:\Users\HP\Documents\UiPath\MatrixAlertAutomation\Data\Capture</t>
+    <t>C:\Users\Rent It\Documents\UiPath\MatrixAlertAutomation\Data\Temp</t>
+  </si>
+  <si>
+    <t>C:\Users\Rent It\Documents\UiPath\MatrixAlertAutomation\Data\Capture</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8">
     <font>
       <sz val="11"/>
@@ -775,16 +775,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1014"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="1" max="1" width="43.5546875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="88.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="88.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -861,7 +861,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="30">
+    <row r="5" spans="1:26" ht="28.8">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -2208,16 +2208,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2254,12 +2254,12 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="28.8">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>24</v>
@@ -3324,12 +3324,12 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.88671875" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" customWidth="1"/>
+    <col min="3" max="3" width="60.33203125" customWidth="1"/>
+    <col min="4" max="26" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
Description : Add arguments Iteration No, Date, Test Case Id, Test Case Step Developer Name : Jagannath Patil Date : 08-Jul-2021
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rent It\Documents\UiPath\MatrixAlertAutomation\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\RTA_Github\MatrixAlertAutomation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="103">
   <si>
     <t>Name</t>
   </si>
@@ -293,9 +293,6 @@
     <t>Step%2020</t>
   </si>
   <si>
-    <t>insyt_web</t>
-  </si>
-  <si>
     <t>RAM_DB</t>
   </si>
   <si>
@@ -327,6 +324,15 @@
   </si>
   <si>
     <t>C:\Users\Rent It\Documents\UiPath\MatrixAlertAutomation\Data\Capture</t>
+  </si>
+  <si>
+    <t>IterationDate</t>
+  </si>
+  <si>
+    <t>IterationNumber</t>
+  </si>
+  <si>
+    <t>ma_web</t>
   </si>
 </sst>
 </file>
@@ -420,7 +426,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -458,6 +464,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -775,16 +782,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1014"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="88.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="88.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -861,7 +868,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="28.8">
+    <row r="5" spans="1:26" ht="30">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -878,10 +885,10 @@
         <v>30</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7" t="s">
         <v>93</v>
-      </c>
-      <c r="C7" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
@@ -998,10 +1005,10 @@
     </row>
     <row r="27" spans="1:3" s="18" customFormat="1" ht="14.25" customHeight="1">
       <c r="A27" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
@@ -1011,10 +1018,10 @@
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B29" s="20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
@@ -1130,7 +1137,7 @@
         <v>76</v>
       </c>
       <c r="B51" s="15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C51" t="s">
         <v>77</v>
@@ -1142,7 +1149,7 @@
         <v>78</v>
       </c>
       <c r="B53" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C53" t="s">
         <v>86</v>
@@ -1223,7 +1230,7 @@
         <v>71</v>
       </c>
       <c r="B75" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="14.25" customHeight="1"/>
@@ -1232,7 +1239,7 @@
         <v>72</v>
       </c>
       <c r="B77" s="14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="14.25" customHeight="1"/>
@@ -1241,7 +1248,7 @@
         <v>73</v>
       </c>
       <c r="B79" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2208,16 +2215,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2254,7 +2261,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2334,8 +2341,22 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>100</v>
+      </c>
+      <c r="B12" s="21">
+        <v>44385</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+    </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
@@ -3324,12 +3345,12 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -3340,7 +3361,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Description : 3rd Release Test Cases - After Dry run in Jagannath Machine Developer Name : Jagannath Patil Date : 04-August-2021
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -320,13 +320,13 @@
     <t>Metrics_Alert_Test Suit</t>
   </si>
   <si>
+    <t>C:\Users\Rent It\Documents\UiPath\MatrixAlertAutomation\Data\Temp\</t>
+  </si>
+  <si>
     <t>Upload_File_path</t>
   </si>
   <si>
-    <t>C:\Users\Rent It\Documents\UiPath\MatrixAlertAutomation\Data\Temp</t>
-  </si>
-  <si>
-    <t>C:\Users\Rent It\Documents\UiPath\MatrixAlertAutomation\Data\Capture</t>
+    <t>C:\Users\Rent It\Documents\Metrics_Alert_project\Data\Capture</t>
   </si>
 </sst>
 </file>
@@ -775,7 +775,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1014"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
@@ -1001,7 +1001,7 @@
         <v>96</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
@@ -1011,7 +1011,7 @@
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" s="19" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B29" s="20" t="s">
         <v>100</v>
@@ -2208,7 +2208,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -2259,7 +2259,7 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>24</v>

</xml_diff>